<commit_message>
Handle read and write file excel
</commit_message>
<xml_diff>
--- a/data/input.xlsx
+++ b/data/input.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4575" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4575"/>
   </bookViews>
   <sheets>
     <sheet name="Basic" sheetId="1" r:id="rId1"/>
@@ -374,8 +374,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:G12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -435,7 +435,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
@@ -458,7 +458,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
         <v>5</v>
@@ -481,7 +481,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B5" t="s">
         <v>0</v>
@@ -504,7 +504,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B6" t="s">
         <v>5</v>
@@ -527,7 +527,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="B7" t="s">
         <v>0</v>
@@ -550,7 +550,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="B8" t="s">
         <v>5</v>
@@ -573,7 +573,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B9" t="s">
         <v>0</v>
@@ -596,7 +596,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="B10" t="s">
         <v>5</v>
@@ -619,7 +619,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="B11" t="s">
         <v>0</v>
@@ -642,7 +642,7 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="B12" t="s">
         <v>5</v>
@@ -672,8 +672,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -733,7 +733,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
@@ -756,7 +756,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
         <v>5</v>
@@ -779,7 +779,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B5" t="s">
         <v>0</v>
@@ -802,7 +802,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B6" t="s">
         <v>5</v>
@@ -825,7 +825,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="B7" t="s">
         <v>0</v>
@@ -848,7 +848,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="B8" t="s">
         <v>5</v>
@@ -871,7 +871,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B9" t="s">
         <v>0</v>
@@ -894,7 +894,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="B10" t="s">
         <v>5</v>
@@ -917,7 +917,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="B11" t="s">
         <v>0</v>
@@ -940,7 +940,7 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="B12" t="s">
         <v>5</v>

</xml_diff>